<commit_message>
hopefully last menu change2
</commit_message>
<xml_diff>
--- a/MenuContent/HotPot_Ingredients_Workbook.xlsx
+++ b/MenuContent/HotPot_Ingredients_Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hot-pot-world-website\Menu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hot-pot-world-website\HotPotWorld\MenuContent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD923AAA-B05D-4AB3-8656-040688461C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8366DC67-754C-493F-A220-20704B3407CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{377B3DF5-2800-4332-8733-1BB2BCABC50E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{377B3DF5-2800-4332-8733-1BB2BCABC50E}"/>
   </bookViews>
   <sheets>
     <sheet name="HotPot_Menu" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="279">
   <si>
     <t>Product_EN</t>
   </si>
@@ -798,6 +798,81 @@
   </si>
   <si>
     <t xml:space="preserve"> MINI SAUSAGES</t>
+  </si>
+  <si>
+    <t>DRINKS</t>
+  </si>
+  <si>
+    <t>NAPOJE</t>
+  </si>
+  <si>
+    <t>PEPSI/PEPSI MAX</t>
+  </si>
+  <si>
+    <t>MIRINDA</t>
+  </si>
+  <si>
+    <t>7UP</t>
+  </si>
+  <si>
+    <t>LIPTON</t>
+  </si>
+  <si>
+    <t>HOMEMADE LEMONADE</t>
+  </si>
+  <si>
+    <t>TOMA JUICE</t>
+  </si>
+  <si>
+    <t>BASIL SEEDS JUICE</t>
+  </si>
+  <si>
+    <t>WATER</t>
+  </si>
+  <si>
+    <t>BUBBLE TEA</t>
+  </si>
+  <si>
+    <t>GUAVA JUICE</t>
+  </si>
+  <si>
+    <t>DOMOWA LEMONIADA</t>
+  </si>
+  <si>
+    <t>SOK Z PESTKAMI BAZYLII</t>
+  </si>
+  <si>
+    <t>WODA</t>
+  </si>
+  <si>
+    <t>SOK Z GUAWY</t>
+  </si>
+  <si>
+    <t>200 ML/500 ML</t>
+  </si>
+  <si>
+    <t>200 ML/1 L</t>
+  </si>
+  <si>
+    <t>400 ML/ 1 L</t>
+  </si>
+  <si>
+    <t>500 ML/1 L</t>
+  </si>
+  <si>
+    <t>8 PLN/10 PLN</t>
+  </si>
+  <si>
+    <t>8 PLN/18 PLN</t>
+  </si>
+  <si>
+    <t>16 PLN/25 PLN</t>
+  </si>
+  <si>
+    <t>8 PLN/16 PLN</t>
+  </si>
+  <si>
+    <t>16 PLN</t>
   </si>
 </sst>
 </file>
@@ -861,7 +936,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -877,9 +952,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -917,7 +992,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -1023,7 +1098,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1193,26 +1268,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E87167-1FB8-4914-8B9E-1A2E468CF660}">
-  <dimension ref="B1:I75"/>
+  <dimension ref="B1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1238,7 +1313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1264,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>75</v>
       </c>
@@ -1290,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>75</v>
       </c>
@@ -1316,7 +1391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -1342,7 +1417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -1368,7 +1443,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>75</v>
       </c>
@@ -1394,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -1420,7 +1495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>75</v>
       </c>
@@ -1446,7 +1521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>75</v>
       </c>
@@ -1472,7 +1547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>75</v>
       </c>
@@ -1498,7 +1573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>74</v>
       </c>
@@ -1524,7 +1599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>74</v>
       </c>
@@ -1550,7 +1625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>74</v>
       </c>
@@ -1576,7 +1651,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>74</v>
       </c>
@@ -1602,7 +1677,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>74</v>
       </c>
@@ -1628,7 +1703,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>74</v>
       </c>
@@ -1654,7 +1729,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>74</v>
       </c>
@@ -1680,7 +1755,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>74</v>
       </c>
@@ -1706,7 +1781,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>74</v>
       </c>
@@ -1732,7 +1807,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
@@ -1758,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>74</v>
       </c>
@@ -1784,7 +1859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -1810,7 +1885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>74</v>
       </c>
@@ -1836,7 +1911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -1862,7 +1937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>74</v>
       </c>
@@ -1888,7 +1963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>74</v>
       </c>
@@ -1914,7 +1989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -1940,7 +2015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>74</v>
       </c>
@@ -1966,7 +2041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>74</v>
       </c>
@@ -1992,7 +2067,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>74</v>
       </c>
@@ -2018,7 +2093,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>74</v>
       </c>
@@ -2044,7 +2119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -2070,7 +2145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>74</v>
       </c>
@@ -2096,7 +2171,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>74</v>
       </c>
@@ -2122,7 +2197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>74</v>
       </c>
@@ -2148,7 +2223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>74</v>
       </c>
@@ -2174,7 +2249,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>74</v>
       </c>
@@ -2200,7 +2275,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>74</v>
       </c>
@@ -2226,7 +2301,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>74</v>
       </c>
@@ -2252,7 +2327,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>74</v>
       </c>
@@ -2278,7 +2353,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>74</v>
       </c>
@@ -2304,7 +2379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>74</v>
       </c>
@@ -2330,7 +2405,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>74</v>
       </c>
@@ -2356,7 +2431,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>74</v>
       </c>
@@ -2382,7 +2457,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>74</v>
       </c>
@@ -2408,7 +2483,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>74</v>
       </c>
@@ -2434,7 +2509,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>74</v>
       </c>
@@ -2460,7 +2535,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>74</v>
       </c>
@@ -2486,7 +2561,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>74</v>
       </c>
@@ -2512,7 +2587,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>74</v>
       </c>
@@ -2538,7 +2613,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>74</v>
       </c>
@@ -2564,7 +2639,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>74</v>
       </c>
@@ -2590,7 +2665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>74</v>
       </c>
@@ -2616,7 +2691,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>74</v>
       </c>
@@ -2642,7 +2717,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>74</v>
       </c>
@@ -2668,7 +2743,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>74</v>
       </c>
@@ -2694,7 +2769,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>74</v>
       </c>
@@ -2720,7 +2795,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>74</v>
       </c>
@@ -2746,7 +2821,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2847,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>74</v>
       </c>
@@ -2798,7 +2873,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>74</v>
       </c>
@@ -2824,7 +2899,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>74</v>
       </c>
@@ -2850,7 +2925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>74</v>
       </c>
@@ -2876,7 +2951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>74</v>
       </c>
@@ -2902,7 +2977,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>74</v>
       </c>
@@ -2928,7 +3003,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>74</v>
       </c>
@@ -2954,7 +3029,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>74</v>
       </c>
@@ -2980,7 +3055,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>74</v>
       </c>
@@ -3006,7 +3081,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>74</v>
       </c>
@@ -3032,7 +3107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>74</v>
       </c>
@@ -3058,7 +3133,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>74</v>
       </c>
@@ -3084,7 +3159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>74</v>
       </c>
@@ -3110,7 +3185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>176</v>
       </c>
@@ -3136,7 +3211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>176</v>
       </c>
@@ -3160,6 +3235,283 @@
       </c>
       <c r="I75" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" t="s">
+        <v>4</v>
+      </c>
+      <c r="H76" t="s">
+        <v>4</v>
+      </c>
+      <c r="I76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>254</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>255</v>
+      </c>
+      <c r="E77" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" t="s">
+        <v>256</v>
+      </c>
+      <c r="G77" t="s">
+        <v>256</v>
+      </c>
+      <c r="H77" t="s">
+        <v>270</v>
+      </c>
+      <c r="I77" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>254</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>255</v>
+      </c>
+      <c r="E78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" t="s">
+        <v>257</v>
+      </c>
+      <c r="G78" t="s">
+        <v>257</v>
+      </c>
+      <c r="H78" t="s">
+        <v>270</v>
+      </c>
+      <c r="I78" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>254</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>255</v>
+      </c>
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" t="s">
+        <v>258</v>
+      </c>
+      <c r="G79" t="s">
+        <v>258</v>
+      </c>
+      <c r="H79" t="s">
+        <v>270</v>
+      </c>
+      <c r="I79" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>254</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>255</v>
+      </c>
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" t="s">
+        <v>259</v>
+      </c>
+      <c r="G80" t="s">
+        <v>259</v>
+      </c>
+      <c r="H80" t="s">
+        <v>270</v>
+      </c>
+      <c r="I80" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>254</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>255</v>
+      </c>
+      <c r="E81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" t="s">
+        <v>261</v>
+      </c>
+      <c r="G81" t="s">
+        <v>261</v>
+      </c>
+      <c r="H81" t="s">
+        <v>271</v>
+      </c>
+      <c r="I81" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>254</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>255</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
+        <v>260</v>
+      </c>
+      <c r="G82" t="s">
+        <v>266</v>
+      </c>
+      <c r="H82" t="s">
+        <v>272</v>
+      </c>
+      <c r="I82" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>255</v>
+      </c>
+      <c r="E83" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" t="s">
+        <v>262</v>
+      </c>
+      <c r="G83" t="s">
+        <v>267</v>
+      </c>
+      <c r="I83" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>254</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>255</v>
+      </c>
+      <c r="E84" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" t="s">
+        <v>263</v>
+      </c>
+      <c r="G84" t="s">
+        <v>268</v>
+      </c>
+      <c r="H84" t="s">
+        <v>273</v>
+      </c>
+      <c r="I84" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>255</v>
+      </c>
+      <c r="E85" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" t="s">
+        <v>264</v>
+      </c>
+      <c r="G85" t="s">
+        <v>264</v>
+      </c>
+      <c r="I85" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>254</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>255</v>
+      </c>
+      <c r="E86" t="s">
+        <v>4</v>
+      </c>
+      <c r="F86" t="s">
+        <v>265</v>
+      </c>
+      <c r="G86" t="s">
+        <v>269</v>
+      </c>
+      <c r="I86" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>